<commit_message>
added visuals for some of the demographics of the programs
</commit_message>
<xml_diff>
--- a/ShinyApp/data/medicaid-enrollment.xlsx
+++ b/ShinyApp/data/medicaid-enrollment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julierebstock/Desktop/Virginia-Tech/DSPG-2021/Loudoun-County/2021_DSPG_Loudoun/ShinyApp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE97FAC6-58EB-5947-8D0D-7F7F2BE573AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C77C2D-5977-4244-82DF-6F41B0FE3AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4120" yWindow="1000" windowWidth="24300" windowHeight="16440" xr2:uid="{EBFEAA5D-9FF0-B149-B5B6-29EF778F4648}"/>
   </bookViews>
@@ -560,7 +560,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,5 +877,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>